<commit_message>
Update design file with questions.
</commit_message>
<xml_diff>
--- a/design/CL-PFU database design.xlsx
+++ b/design/CL-PFU database design.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/TestTargetsDB/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2DE0FE-99FF-4C48-A760-86695D9A9A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DBE15F-0F20-BF4F-B457-98C7C05C553A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="500" windowWidth="41400" windowHeight="28120" xr2:uid="{7D1B523B-6A41-0844-B2C9-E0154220E900}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{7D1B523B-6A41-0844-B2C9-E0154220E900}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Design" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -169,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="598">
   <si>
     <t>Energy</t>
   </si>
@@ -1948,6 +1949,21 @@
   </si>
   <si>
     <t>CompletedEfficiencies</t>
+  </si>
+  <si>
+    <t>* Is there a PostgreSQL command that returns the primary key and foreign keys for a table?</t>
+  </si>
+  <si>
+    <t>* How do we handle foreign key columns that have different meaning in a table?</t>
+  </si>
+  <si>
+    <t>There can be multiple versions of the same foreign key with different meanings.</t>
+  </si>
+  <si>
+    <t>* If we split all data into multiple tables, how can we make a table that has the values of the keys, not the integer keys themselves?</t>
+  </si>
+  <si>
+    <t>Is it a matter of doing a series of joins? That seems tedious.</t>
   </si>
 </sst>
 </file>
@@ -2049,25 +2065,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2083,8 +2093,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2403,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1652E8C3-254B-7F40-96D6-2C741A6B398E}">
   <dimension ref="A2:DJ184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CJ1" workbookViewId="0">
+    <sheetView topLeftCell="CJ1" workbookViewId="0">
       <selection activeCell="BU10" sqref="BU10"/>
     </sheetView>
   </sheetViews>
@@ -2453,7 +2465,7 @@
       </c>
     </row>
     <row r="3" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -2461,138 +2473,138 @@
       </c>
     </row>
     <row r="8" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="K8" s="14" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="K8" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="AA8" s="14" t="s">
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="AA8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="AB8" s="14"/>
-      <c r="AD8" s="14" t="s">
+      <c r="AB8" s="11"/>
+      <c r="AD8" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="AE8" s="14"/>
-      <c r="AG8" s="14" t="s">
+      <c r="AE8" s="11"/>
+      <c r="AG8" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="AH8" s="14"/>
-      <c r="AI8" s="14"/>
-      <c r="AK8" s="14" t="s">
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AK8" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="AL8" s="14"/>
-      <c r="AN8" s="14" t="s">
+      <c r="AL8" s="11"/>
+      <c r="AN8" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="AO8" s="14"/>
-      <c r="AQ8" s="14" t="s">
+      <c r="AO8" s="11"/>
+      <c r="AQ8" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="AR8" s="14"/>
-      <c r="AS8" s="14"/>
+      <c r="AR8" s="11"/>
+      <c r="AS8" s="11"/>
       <c r="AU8" t="s">
         <v>374</v>
       </c>
-      <c r="AZ8" s="3" t="s">
+      <c r="AZ8" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="BA8" s="3"/>
-      <c r="BB8" s="3"/>
-      <c r="BD8" s="14" t="s">
+      <c r="BA8" s="12"/>
+      <c r="BB8" s="12"/>
+      <c r="BD8" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="BE8" s="14"/>
-      <c r="BG8" s="14" t="s">
+      <c r="BE8" s="11"/>
+      <c r="BG8" s="11" t="s">
         <v>506</v>
       </c>
-      <c r="BH8" s="14"/>
+      <c r="BH8" s="11"/>
       <c r="BI8" s="2"/>
-      <c r="BJ8" s="14" t="s">
+      <c r="BJ8" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="BK8" s="14"/>
+      <c r="BK8" s="11"/>
       <c r="BL8" s="2"/>
-      <c r="BM8" s="14" t="s">
+      <c r="BM8" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="BN8" s="14"/>
-      <c r="BP8" s="14" t="s">
+      <c r="BN8" s="11"/>
+      <c r="BP8" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="BQ8" s="14"/>
-      <c r="BR8" s="14"/>
-      <c r="BS8" s="14"/>
-      <c r="BT8" s="14"/>
-      <c r="BU8" s="14"/>
-      <c r="BV8" s="14"/>
-      <c r="BW8" s="14"/>
-      <c r="BX8" s="14"/>
-      <c r="BY8" s="14"/>
-      <c r="BZ8" s="14"/>
-      <c r="CA8" s="14"/>
-      <c r="CB8" s="14"/>
-      <c r="CC8" s="14"/>
-      <c r="CD8" s="14"/>
-      <c r="CE8" s="14"/>
-      <c r="CG8" s="14" t="s">
+      <c r="BQ8" s="11"/>
+      <c r="BR8" s="11"/>
+      <c r="BS8" s="11"/>
+      <c r="BT8" s="11"/>
+      <c r="BU8" s="11"/>
+      <c r="BV8" s="11"/>
+      <c r="BW8" s="11"/>
+      <c r="BX8" s="11"/>
+      <c r="BY8" s="11"/>
+      <c r="BZ8" s="11"/>
+      <c r="CA8" s="11"/>
+      <c r="CB8" s="11"/>
+      <c r="CC8" s="11"/>
+      <c r="CD8" s="11"/>
+      <c r="CE8" s="11"/>
+      <c r="CG8" s="11" t="s">
         <v>586</v>
       </c>
-      <c r="CH8" s="14"/>
-      <c r="CJ8" s="14" t="s">
+      <c r="CH8" s="11"/>
+      <c r="CJ8" s="11" t="s">
         <v>591</v>
       </c>
-      <c r="CK8" s="14"/>
-      <c r="CL8" s="14"/>
-      <c r="CM8" s="14"/>
-      <c r="CN8" s="14"/>
-      <c r="CO8" s="14"/>
-      <c r="CP8" s="14"/>
-      <c r="CQ8" s="14"/>
-      <c r="CR8" s="14"/>
-      <c r="CS8" s="14"/>
-      <c r="CT8" s="14"/>
-      <c r="CU8" s="14"/>
-      <c r="CV8" s="14"/>
-      <c r="CW8" s="14"/>
-      <c r="CX8" s="14"/>
-      <c r="CZ8" s="14" t="s">
+      <c r="CK8" s="11"/>
+      <c r="CL8" s="11"/>
+      <c r="CM8" s="11"/>
+      <c r="CN8" s="11"/>
+      <c r="CO8" s="11"/>
+      <c r="CP8" s="11"/>
+      <c r="CQ8" s="11"/>
+      <c r="CR8" s="11"/>
+      <c r="CS8" s="11"/>
+      <c r="CT8" s="11"/>
+      <c r="CU8" s="11"/>
+      <c r="CV8" s="11"/>
+      <c r="CW8" s="11"/>
+      <c r="CX8" s="11"/>
+      <c r="CZ8" s="11" t="s">
         <v>592</v>
       </c>
-      <c r="DA8" s="14"/>
-      <c r="DB8" s="14"/>
-      <c r="DC8" s="14"/>
-      <c r="DD8" s="14"/>
-      <c r="DE8" s="14"/>
-      <c r="DF8" s="14"/>
-      <c r="DG8" s="14"/>
-      <c r="DH8" s="14"/>
-      <c r="DI8" s="14"/>
-      <c r="DJ8" s="14"/>
+      <c r="DA8" s="11"/>
+      <c r="DB8" s="11"/>
+      <c r="DC8" s="11"/>
+      <c r="DD8" s="11"/>
+      <c r="DE8" s="11"/>
+      <c r="DF8" s="11"/>
+      <c r="DG8" s="11"/>
+      <c r="DH8" s="11"/>
+      <c r="DI8" s="11"/>
+      <c r="DJ8" s="11"/>
     </row>
     <row r="9" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -2625,46 +2637,46 @@
       <c r="K9" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="Q9" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="S9" s="5" t="s">
+      <c r="S9" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="T9" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="U9" s="5" t="s">
+      <c r="U9" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="V9" s="5" t="s">
+      <c r="V9" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="W9" s="5" t="s">
+      <c r="W9" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="X9" s="5" t="s">
+      <c r="X9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Y9" s="5" t="s">
+      <c r="Y9" s="4" t="s">
         <v>183</v>
       </c>
       <c r="AA9" s="1" t="s">
@@ -2673,10 +2685,10 @@
       <c r="AB9" t="s">
         <v>4</v>
       </c>
-      <c r="AD9" s="7" t="s">
+      <c r="AD9" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="AE9" s="6" t="s">
+      <c r="AE9" s="3" t="s">
         <v>193</v>
       </c>
       <c r="AG9" s="1" t="s">
@@ -2706,7 +2718,7 @@
       <c r="AR9" t="s">
         <v>244</v>
       </c>
-      <c r="AS9" s="10" t="s">
+      <c r="AS9" s="8" t="s">
         <v>375</v>
       </c>
       <c r="AU9" s="1" t="s">
@@ -2721,7 +2733,7 @@
       <c r="BA9" t="s">
         <v>246</v>
       </c>
-      <c r="BB9" s="10" t="s">
+      <c r="BB9" s="8" t="s">
         <v>364</v>
       </c>
       <c r="BD9" s="1" t="s">
@@ -2751,43 +2763,43 @@
       <c r="BQ9" t="s">
         <v>502</v>
       </c>
-      <c r="BR9" s="10" t="s">
+      <c r="BR9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="BS9" s="10" t="s">
+      <c r="BS9" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="BT9" s="10" t="s">
+      <c r="BT9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="BU9" s="13" t="s">
+      <c r="BU9" t="s">
         <v>207</v>
       </c>
-      <c r="BV9" s="10" t="s">
+      <c r="BV9" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="BW9" s="13" t="s">
+      <c r="BW9" t="s">
         <v>506</v>
       </c>
-      <c r="BX9" s="13" t="s">
+      <c r="BX9" t="s">
         <v>514</v>
       </c>
-      <c r="BY9" s="13" t="s">
+      <c r="BY9" t="s">
         <v>567</v>
       </c>
-      <c r="BZ9" s="13" t="s">
+      <c r="BZ9" t="s">
         <v>566</v>
       </c>
-      <c r="CA9" s="10" t="s">
+      <c r="CA9" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="CB9" s="13" t="s">
+      <c r="CB9" t="s">
         <v>503</v>
       </c>
-      <c r="CC9" s="13" t="s">
+      <c r="CC9" t="s">
         <v>504</v>
       </c>
-      <c r="CD9" s="13" t="s">
+      <c r="CD9" t="s">
         <v>570</v>
       </c>
       <c r="CE9" t="s">
@@ -2859,22 +2871,22 @@
       <c r="DD9" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="DE9" s="13" t="s">
+      <c r="DE9" t="s">
         <v>574</v>
       </c>
-      <c r="DF9" s="13" t="s">
+      <c r="DF9" t="s">
         <v>578</v>
       </c>
-      <c r="DG9" s="13" t="s">
+      <c r="DG9" t="s">
         <v>573</v>
       </c>
-      <c r="DH9" s="13" t="s">
+      <c r="DH9" t="s">
         <v>502</v>
       </c>
-      <c r="DI9" s="13" t="s">
+      <c r="DI9" t="s">
         <v>505</v>
       </c>
-      <c r="DJ9" s="13" t="s">
+      <c r="DJ9" t="s">
         <v>589</v>
       </c>
     </row>
@@ -2948,7 +2960,7 @@
       <c r="AR10" t="s">
         <v>376</v>
       </c>
-      <c r="AS10" s="10"/>
+      <c r="AS10" s="8"/>
       <c r="AU10" s="1">
         <v>1</v>
       </c>
@@ -2958,16 +2970,16 @@
       <c r="AZ10" s="1">
         <v>1</v>
       </c>
-      <c r="BA10" s="4" t="s">
+      <c r="BA10" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="BB10" s="11" t="s">
+      <c r="BB10" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD10" s="1">
         <v>1</v>
       </c>
-      <c r="BE10" s="4" t="s">
+      <c r="BE10" s="3" t="s">
         <v>316</v>
       </c>
       <c r="BG10" s="1">
@@ -2991,35 +3003,35 @@
       <c r="BP10" s="1">
         <v>1</v>
       </c>
-      <c r="BR10" s="10" t="s">
+      <c r="BR10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="BS10" s="10"/>
-      <c r="BT10" s="10"/>
-      <c r="BU10" s="13" t="s">
+      <c r="BS10" s="8"/>
+      <c r="BT10" s="8"/>
+      <c r="BU10" t="s">
         <v>227</v>
       </c>
-      <c r="BV10" s="10"/>
-      <c r="BW10" s="13" t="s">
+      <c r="BV10" s="8"/>
+      <c r="BW10" t="s">
         <v>568</v>
       </c>
-      <c r="BX10" s="13" t="s">
+      <c r="BX10" t="s">
         <v>227</v>
       </c>
-      <c r="BY10" s="13" t="s">
+      <c r="BY10" t="s">
         <v>227</v>
       </c>
-      <c r="BZ10" s="13" t="s">
+      <c r="BZ10" t="s">
         <v>227</v>
       </c>
-      <c r="CA10" s="10"/>
-      <c r="CB10" s="13" t="s">
+      <c r="CA10" s="8"/>
+      <c r="CB10" t="s">
         <v>227</v>
       </c>
-      <c r="CC10" s="13" t="s">
+      <c r="CC10" t="s">
         <v>227</v>
       </c>
-      <c r="CD10" s="13" t="b">
+      <c r="CD10" t="b">
         <v>1</v>
       </c>
       <c r="CG10" s="1">
@@ -3146,7 +3158,7 @@
       <c r="AR11" t="s">
         <v>377</v>
       </c>
-      <c r="AS11" s="10"/>
+      <c r="AS11" s="8"/>
       <c r="AU11" s="1">
         <v>2</v>
       </c>
@@ -3156,16 +3168,16 @@
       <c r="AZ11" s="1">
         <v>2</v>
       </c>
-      <c r="BA11" s="4" t="s">
+      <c r="BA11" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="BB11" s="11" t="s">
+      <c r="BB11" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD11" s="1">
         <v>2</v>
       </c>
-      <c r="BE11" s="4" t="s">
+      <c r="BE11" s="3" t="s">
         <v>317</v>
       </c>
       <c r="BG11" s="1">
@@ -3189,35 +3201,35 @@
       <c r="BP11" s="1">
         <v>2</v>
       </c>
-      <c r="BR11" s="10" t="s">
+      <c r="BR11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="BS11" s="10"/>
-      <c r="BT11" s="10"/>
-      <c r="BU11" s="13" t="s">
+      <c r="BS11" s="8"/>
+      <c r="BT11" s="8"/>
+      <c r="BU11" t="s">
         <v>590</v>
       </c>
-      <c r="BV11" s="10"/>
-      <c r="BW11" s="13" t="s">
+      <c r="BV11" s="8"/>
+      <c r="BW11" t="s">
         <v>569</v>
       </c>
-      <c r="BX11" s="13" t="s">
+      <c r="BX11" t="s">
         <v>247</v>
       </c>
-      <c r="BY11" s="13" t="s">
+      <c r="BY11" t="s">
         <v>513</v>
       </c>
-      <c r="BZ11" s="13" t="s">
+      <c r="BZ11" t="s">
         <v>513</v>
       </c>
-      <c r="CA11" s="10"/>
-      <c r="CB11" s="13" t="s">
+      <c r="CA11" s="8"/>
+      <c r="CB11" t="s">
         <v>245</v>
       </c>
-      <c r="CC11" s="13" t="s">
+      <c r="CC11" t="s">
         <v>247</v>
       </c>
-      <c r="CD11" s="13" t="b">
+      <c r="CD11" t="b">
         <v>0</v>
       </c>
       <c r="CG11" s="1">
@@ -3335,7 +3347,7 @@
       <c r="AR12" t="s">
         <v>378</v>
       </c>
-      <c r="AS12" s="10"/>
+      <c r="AS12" s="8"/>
       <c r="AU12" s="1">
         <v>3</v>
       </c>
@@ -3345,16 +3357,16 @@
       <c r="AZ12" s="1">
         <v>3</v>
       </c>
-      <c r="BA12" s="4" t="s">
+      <c r="BA12" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="BB12" s="11" t="s">
+      <c r="BB12" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD12" s="1">
         <v>3</v>
       </c>
-      <c r="BE12" s="4" t="s">
+      <c r="BE12" s="3" t="s">
         <v>267</v>
       </c>
       <c r="BG12" s="1">
@@ -3378,21 +3390,13 @@
       <c r="BP12" s="1">
         <v>3</v>
       </c>
-      <c r="BR12" s="10" t="s">
+      <c r="BR12" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="BS12" s="10"/>
-      <c r="BT12" s="10"/>
-      <c r="BU12" s="13"/>
-      <c r="BV12" s="10"/>
-      <c r="BW12" s="13"/>
-      <c r="BX12" s="13"/>
-      <c r="BY12" s="13"/>
-      <c r="BZ12" s="13"/>
-      <c r="CA12" s="10"/>
-      <c r="CB12" s="13"/>
-      <c r="CC12" s="13"/>
-      <c r="CD12" s="13"/>
+      <c r="BS12" s="8"/>
+      <c r="BT12" s="8"/>
+      <c r="BV12" s="8"/>
+      <c r="CA12" s="8"/>
       <c r="CJ12" s="1">
         <v>3</v>
       </c>
@@ -3460,7 +3464,7 @@
       <c r="AR13" t="s">
         <v>560</v>
       </c>
-      <c r="AS13" s="10"/>
+      <c r="AS13" s="8"/>
       <c r="AU13" s="1">
         <v>4</v>
       </c>
@@ -3470,16 +3474,16 @@
       <c r="AZ13" s="1">
         <v>4</v>
       </c>
-      <c r="BA13" s="4" t="s">
+      <c r="BA13" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="BB13" s="11" t="s">
+      <c r="BB13" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD13" s="1">
         <v>4</v>
       </c>
-      <c r="BE13" s="4" t="s">
+      <c r="BE13" s="3" t="s">
         <v>318</v>
       </c>
       <c r="BJ13" s="1">
@@ -3491,21 +3495,13 @@
       <c r="BP13" s="1">
         <v>4</v>
       </c>
-      <c r="BR13" s="10" t="s">
+      <c r="BR13" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="BS13" s="10"/>
-      <c r="BT13" s="10"/>
-      <c r="BU13" s="13"/>
-      <c r="BV13" s="10"/>
-      <c r="BW13" s="13"/>
-      <c r="BX13" s="13"/>
-      <c r="BY13" s="13"/>
-      <c r="BZ13" s="13"/>
-      <c r="CA13" s="10"/>
-      <c r="CB13" s="13"/>
-      <c r="CC13" s="13"/>
-      <c r="CD13" s="13"/>
+      <c r="BS13" s="8"/>
+      <c r="BT13" s="8"/>
+      <c r="BV13" s="8"/>
+      <c r="CA13" s="8"/>
     </row>
     <row r="14" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -3556,26 +3552,26 @@
       <c r="AR14" t="s">
         <v>561</v>
       </c>
-      <c r="AS14" s="10"/>
+      <c r="AS14" s="8"/>
       <c r="AU14" s="1">
         <v>5</v>
       </c>
-      <c r="AV14" s="4" t="s">
+      <c r="AV14" s="3" t="s">
         <v>478</v>
       </c>
       <c r="AZ14" s="1">
         <v>5</v>
       </c>
-      <c r="BA14" s="4" t="s">
+      <c r="BA14" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="BB14" s="11" t="s">
+      <c r="BB14" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD14" s="1">
         <v>5</v>
       </c>
-      <c r="BE14" s="4" t="s">
+      <c r="BE14" s="3" t="s">
         <v>319</v>
       </c>
       <c r="BJ14" s="1">
@@ -3587,21 +3583,13 @@
       <c r="BP14" s="1">
         <v>5</v>
       </c>
-      <c r="BR14" s="10" t="s">
+      <c r="BR14" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="BS14" s="10"/>
-      <c r="BT14" s="10"/>
-      <c r="BU14" s="13"/>
-      <c r="BV14" s="10"/>
-      <c r="BW14" s="13"/>
-      <c r="BX14" s="13"/>
-      <c r="BY14" s="13"/>
-      <c r="BZ14" s="13"/>
-      <c r="CA14" s="10"/>
-      <c r="CB14" s="13"/>
-      <c r="CC14" s="13"/>
-      <c r="CD14" s="13"/>
+      <c r="BS14" s="8"/>
+      <c r="BT14" s="8"/>
+      <c r="BV14" s="8"/>
+      <c r="CA14" s="8"/>
     </row>
     <row r="15" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -3646,26 +3634,26 @@
       <c r="AR15" t="s">
         <v>562</v>
       </c>
-      <c r="AS15" s="10"/>
+      <c r="AS15" s="8"/>
       <c r="AU15" s="1">
         <v>6</v>
       </c>
-      <c r="AV15" s="4" t="s">
+      <c r="AV15" s="3" t="s">
         <v>479</v>
       </c>
       <c r="AZ15" s="1">
         <v>6</v>
       </c>
-      <c r="BA15" s="4" t="s">
+      <c r="BA15" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="BB15" s="11" t="s">
+      <c r="BB15" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD15" s="1">
         <v>6</v>
       </c>
-      <c r="BE15" s="4" t="s">
+      <c r="BE15" s="3" t="s">
         <v>313</v>
       </c>
       <c r="BJ15" s="1">
@@ -3677,21 +3665,13 @@
       <c r="BP15" s="1">
         <v>6</v>
       </c>
-      <c r="BR15" s="10" t="s">
+      <c r="BR15" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="BS15" s="10"/>
-      <c r="BT15" s="10"/>
-      <c r="BU15" s="13"/>
-      <c r="BV15" s="10"/>
-      <c r="BW15" s="13"/>
-      <c r="BX15" s="13"/>
-      <c r="BY15" s="13"/>
-      <c r="BZ15" s="13"/>
-      <c r="CA15" s="10"/>
-      <c r="CB15" s="13"/>
-      <c r="CC15" s="13"/>
-      <c r="CD15" s="13"/>
+      <c r="BS15" s="8"/>
+      <c r="BT15" s="8"/>
+      <c r="BV15" s="8"/>
+      <c r="CA15" s="8"/>
     </row>
     <row r="16" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -3736,26 +3716,26 @@
       <c r="AR16" t="s">
         <v>381</v>
       </c>
-      <c r="AS16" s="10"/>
+      <c r="AS16" s="8"/>
       <c r="AU16" s="1">
         <v>7</v>
       </c>
-      <c r="AV16" s="4" t="s">
+      <c r="AV16" s="3" t="s">
         <v>498</v>
       </c>
       <c r="AZ16" s="1">
         <v>7</v>
       </c>
-      <c r="BA16" s="4" t="s">
+      <c r="BA16" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="BB16" s="11" t="s">
+      <c r="BB16" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD16" s="1">
         <v>7</v>
       </c>
-      <c r="BE16" s="4" t="s">
+      <c r="BE16" s="3" t="s">
         <v>312</v>
       </c>
       <c r="BJ16" s="1">
@@ -3767,21 +3747,13 @@
       <c r="BP16" s="1">
         <v>7</v>
       </c>
-      <c r="BR16" s="10" t="s">
+      <c r="BR16" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="BS16" s="10"/>
-      <c r="BT16" s="10"/>
-      <c r="BU16" s="13"/>
-      <c r="BV16" s="10"/>
-      <c r="BW16" s="13"/>
-      <c r="BX16" s="13"/>
-      <c r="BY16" s="13"/>
-      <c r="BZ16" s="13"/>
-      <c r="CA16" s="10"/>
-      <c r="CB16" s="13"/>
-      <c r="CC16" s="13"/>
-      <c r="CD16" s="13"/>
+      <c r="BS16" s="8"/>
+      <c r="BT16" s="8"/>
+      <c r="BV16" s="8"/>
+      <c r="CA16" s="8"/>
     </row>
     <row r="17" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -3826,26 +3798,26 @@
       <c r="AR17" t="s">
         <v>382</v>
       </c>
-      <c r="AS17" s="10"/>
+      <c r="AS17" s="8"/>
       <c r="AU17" s="1">
         <v>8</v>
       </c>
-      <c r="AV17" s="4" t="s">
+      <c r="AV17" s="3" t="s">
         <v>500</v>
       </c>
       <c r="AZ17" s="1">
         <v>8</v>
       </c>
-      <c r="BA17" s="4" t="s">
+      <c r="BA17" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="BB17" s="11" t="s">
+      <c r="BB17" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD17" s="1">
         <v>8</v>
       </c>
-      <c r="BE17" s="8" t="s">
+      <c r="BE17" s="6" t="s">
         <v>314</v>
       </c>
       <c r="BJ17" s="1">
@@ -3857,14 +3829,13 @@
       <c r="BP17" s="1">
         <v>8</v>
       </c>
-      <c r="BR17" s="10" t="s">
+      <c r="BR17" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="BS17" s="10"/>
-      <c r="BT17" s="10"/>
-      <c r="BU17" s="13"/>
-      <c r="BV17" s="10"/>
-      <c r="CA17" s="10"/>
+      <c r="BS17" s="8"/>
+      <c r="BT17" s="8"/>
+      <c r="BV17" s="8"/>
+      <c r="CA17" s="8"/>
     </row>
     <row r="18" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -3909,39 +3880,38 @@
       <c r="AR18" t="s">
         <v>383</v>
       </c>
-      <c r="AS18" s="10"/>
+      <c r="AS18" s="8"/>
       <c r="AU18" s="1">
         <v>9</v>
       </c>
-      <c r="AV18" s="4" t="s">
+      <c r="AV18" s="3" t="s">
         <v>499</v>
       </c>
       <c r="AZ18" s="1">
         <v>9</v>
       </c>
-      <c r="BA18" s="4" t="s">
+      <c r="BA18" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="BB18" s="11" t="s">
+      <c r="BB18" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD18" s="1">
         <v>9</v>
       </c>
-      <c r="BE18" s="8" t="s">
+      <c r="BE18" s="6" t="s">
         <v>315</v>
       </c>
       <c r="BP18" s="1">
         <v>9</v>
       </c>
-      <c r="BR18" s="10" t="s">
+      <c r="BR18" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="BS18" s="10"/>
-      <c r="BT18" s="10"/>
-      <c r="BU18" s="13"/>
-      <c r="BV18" s="10"/>
-      <c r="CA18" s="10"/>
+      <c r="BS18" s="8"/>
+      <c r="BT18" s="8"/>
+      <c r="BV18" s="8"/>
+      <c r="CA18" s="8"/>
     </row>
     <row r="19" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -3986,33 +3956,32 @@
       <c r="AR19" t="s">
         <v>384</v>
       </c>
-      <c r="AS19" s="10"/>
+      <c r="AS19" s="8"/>
       <c r="AZ19" s="1">
         <v>10</v>
       </c>
-      <c r="BA19" s="4" t="s">
+      <c r="BA19" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="BB19" s="11" t="s">
+      <c r="BB19" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD19" s="1">
         <v>10</v>
       </c>
-      <c r="BE19" s="4" t="s">
+      <c r="BE19" s="3" t="s">
         <v>344</v>
       </c>
       <c r="BP19" s="1">
         <v>10</v>
       </c>
-      <c r="BR19" s="10" t="s">
+      <c r="BR19" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="BS19" s="10"/>
-      <c r="BT19" s="10"/>
-      <c r="BU19" s="13"/>
-      <c r="BV19" s="10"/>
-      <c r="CA19" s="10"/>
+      <c r="BS19" s="8"/>
+      <c r="BT19" s="8"/>
+      <c r="BV19" s="8"/>
+      <c r="CA19" s="8"/>
     </row>
     <row r="20" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -4057,33 +4026,32 @@
       <c r="AR20" t="s">
         <v>385</v>
       </c>
-      <c r="AS20" s="10"/>
+      <c r="AS20" s="8"/>
       <c r="AZ20" s="1">
         <v>11</v>
       </c>
-      <c r="BA20" s="4" t="s">
+      <c r="BA20" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="BB20" s="11" t="s">
+      <c r="BB20" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD20" s="1">
         <v>11</v>
       </c>
-      <c r="BE20" s="4" t="s">
+      <c r="BE20" s="3" t="s">
         <v>321</v>
       </c>
       <c r="BP20" s="1">
         <v>11</v>
       </c>
-      <c r="BR20" s="10" t="s">
+      <c r="BR20" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="BS20" s="10"/>
-      <c r="BT20" s="10"/>
-      <c r="BU20" s="13"/>
-      <c r="BV20" s="10"/>
-      <c r="CA20" s="10"/>
+      <c r="BS20" s="8"/>
+      <c r="BT20" s="8"/>
+      <c r="BV20" s="8"/>
+      <c r="CA20" s="8"/>
     </row>
     <row r="21" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -4128,35 +4096,34 @@
       <c r="AR21" t="s">
         <v>379</v>
       </c>
-      <c r="AS21" s="11" t="s">
+      <c r="AS21" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ21" s="1">
         <v>12</v>
       </c>
-      <c r="BA21" s="4" t="s">
+      <c r="BA21" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="BB21" s="11" t="s">
+      <c r="BB21" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD21" s="1">
         <v>12</v>
       </c>
-      <c r="BE21" s="4" t="s">
+      <c r="BE21" s="3" t="s">
         <v>323</v>
       </c>
       <c r="BP21" s="1">
         <v>12</v>
       </c>
-      <c r="BR21" s="10" t="s">
+      <c r="BR21" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="BS21" s="10"/>
-      <c r="BT21" s="10"/>
-      <c r="BU21" s="13"/>
-      <c r="BV21" s="10"/>
-      <c r="CA21" s="10"/>
+      <c r="BS21" s="8"/>
+      <c r="BT21" s="8"/>
+      <c r="BV21" s="8"/>
+      <c r="CA21" s="8"/>
     </row>
     <row r="22" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -4201,35 +4168,34 @@
       <c r="AR22" t="s">
         <v>386</v>
       </c>
-      <c r="AS22" s="11" t="s">
+      <c r="AS22" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ22" s="1">
         <v>13</v>
       </c>
-      <c r="BA22" s="4" t="s">
+      <c r="BA22" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="BB22" s="11" t="s">
+      <c r="BB22" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD22" s="1">
         <v>13</v>
       </c>
-      <c r="BE22" s="4" t="s">
+      <c r="BE22" s="3" t="s">
         <v>327</v>
       </c>
       <c r="BP22" s="1">
         <v>13</v>
       </c>
-      <c r="BR22" s="10" t="s">
+      <c r="BR22" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="BS22" s="10"/>
-      <c r="BT22" s="10"/>
-      <c r="BU22" s="13"/>
-      <c r="BV22" s="10"/>
-      <c r="CA22" s="10"/>
+      <c r="BS22" s="8"/>
+      <c r="BT22" s="8"/>
+      <c r="BV22" s="8"/>
+      <c r="CA22" s="8"/>
     </row>
     <row r="23" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -4274,35 +4240,34 @@
       <c r="AR23" t="s">
         <v>387</v>
       </c>
-      <c r="AS23" s="11" t="s">
+      <c r="AS23" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ23" s="1">
         <v>14</v>
       </c>
-      <c r="BA23" s="4" t="s">
+      <c r="BA23" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="BB23" s="11" t="s">
+      <c r="BB23" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD23" s="1">
         <v>14</v>
       </c>
-      <c r="BE23" s="4" t="s">
+      <c r="BE23" s="3" t="s">
         <v>349</v>
       </c>
       <c r="BP23" s="1">
         <v>14</v>
       </c>
-      <c r="BR23" s="10" t="s">
+      <c r="BR23" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="BS23" s="10"/>
-      <c r="BT23" s="10"/>
-      <c r="BU23" s="13"/>
-      <c r="BV23" s="10"/>
-      <c r="CA23" s="10"/>
+      <c r="BS23" s="8"/>
+      <c r="BT23" s="8"/>
+      <c r="BV23" s="8"/>
+      <c r="CA23" s="8"/>
     </row>
     <row r="24" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -4347,35 +4312,34 @@
       <c r="AR24" t="s">
         <v>388</v>
       </c>
-      <c r="AS24" s="11" t="s">
+      <c r="AS24" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ24" s="1">
         <v>15</v>
       </c>
-      <c r="BA24" s="4" t="s">
+      <c r="BA24" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="BB24" s="11" t="s">
+      <c r="BB24" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD24" s="1">
         <v>15</v>
       </c>
-      <c r="BE24" s="4" t="s">
+      <c r="BE24" s="3" t="s">
         <v>340</v>
       </c>
       <c r="BP24" s="1">
         <v>15</v>
       </c>
-      <c r="BR24" s="10" t="s">
+      <c r="BR24" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="BS24" s="10"/>
-      <c r="BT24" s="10"/>
-      <c r="BU24" s="13"/>
-      <c r="BV24" s="10"/>
-      <c r="CA24" s="10"/>
+      <c r="BS24" s="8"/>
+      <c r="BT24" s="8"/>
+      <c r="BV24" s="8"/>
+      <c r="CA24" s="8"/>
     </row>
     <row r="25" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -4420,35 +4384,34 @@
       <c r="AR25" t="s">
         <v>389</v>
       </c>
-      <c r="AS25" s="11" t="s">
+      <c r="AS25" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ25" s="1">
         <v>16</v>
       </c>
-      <c r="BA25" s="4" t="s">
+      <c r="BA25" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="BB25" s="11" t="s">
+      <c r="BB25" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD25" s="1">
         <v>16</v>
       </c>
-      <c r="BE25" s="4" t="s">
+      <c r="BE25" s="3" t="s">
         <v>337</v>
       </c>
       <c r="BP25" s="1">
         <v>16</v>
       </c>
-      <c r="BR25" s="10" t="s">
+      <c r="BR25" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="BS25" s="10"/>
-      <c r="BT25" s="10"/>
-      <c r="BU25" s="13"/>
-      <c r="BV25" s="10"/>
-      <c r="CA25" s="10"/>
+      <c r="BS25" s="8"/>
+      <c r="BT25" s="8"/>
+      <c r="BV25" s="8"/>
+      <c r="CA25" s="8"/>
     </row>
     <row r="26" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -4493,35 +4456,34 @@
       <c r="AR26" t="s">
         <v>516</v>
       </c>
-      <c r="AS26" s="11" t="s">
+      <c r="AS26" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ26" s="1">
         <v>17</v>
       </c>
-      <c r="BA26" s="4" t="s">
+      <c r="BA26" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="BB26" s="11" t="s">
+      <c r="BB26" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD26" s="1">
         <v>17</v>
       </c>
-      <c r="BE26" s="4" t="s">
+      <c r="BE26" s="3" t="s">
         <v>335</v>
       </c>
       <c r="BP26" s="1">
         <v>17</v>
       </c>
-      <c r="BR26" s="10" t="s">
+      <c r="BR26" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="BS26" s="10"/>
-      <c r="BT26" s="10"/>
-      <c r="BU26" s="13"/>
-      <c r="BV26" s="10"/>
-      <c r="CA26" s="10"/>
+      <c r="BS26" s="8"/>
+      <c r="BT26" s="8"/>
+      <c r="BV26" s="8"/>
+      <c r="CA26" s="8"/>
     </row>
     <row r="27" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -4566,35 +4528,34 @@
       <c r="AR27" t="s">
         <v>517</v>
       </c>
-      <c r="AS27" s="11" t="s">
+      <c r="AS27" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ27" s="1">
         <v>18</v>
       </c>
-      <c r="BA27" s="4" t="s">
+      <c r="BA27" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="BB27" s="11" t="s">
+      <c r="BB27" s="9" t="s">
         <v>316</v>
       </c>
       <c r="BD27" s="1">
         <v>18</v>
       </c>
-      <c r="BE27" s="4" t="s">
+      <c r="BE27" s="3" t="s">
         <v>334</v>
       </c>
       <c r="BP27" s="1">
         <v>18</v>
       </c>
-      <c r="BR27" s="10" t="s">
+      <c r="BR27" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="BS27" s="10"/>
-      <c r="BT27" s="10"/>
-      <c r="BU27" s="13"/>
-      <c r="BV27" s="10"/>
-      <c r="CA27" s="10"/>
+      <c r="BS27" s="8"/>
+      <c r="BT27" s="8"/>
+      <c r="BV27" s="8"/>
+      <c r="CA27" s="8"/>
     </row>
     <row r="28" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -4639,35 +4600,34 @@
       <c r="AR28" t="s">
         <v>518</v>
       </c>
-      <c r="AS28" s="11" t="s">
+      <c r="AS28" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ28" s="1">
         <v>19</v>
       </c>
-      <c r="BA28" s="8" t="s">
+      <c r="BA28" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="BB28" s="11" t="s">
+      <c r="BB28" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BD28" s="1">
         <v>19</v>
       </c>
-      <c r="BE28" s="4" t="s">
+      <c r="BE28" s="3" t="s">
         <v>357</v>
       </c>
       <c r="BP28" s="1">
         <v>19</v>
       </c>
-      <c r="BR28" s="10" t="s">
+      <c r="BR28" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="BS28" s="10"/>
-      <c r="BT28" s="10"/>
-      <c r="BU28" s="13"/>
-      <c r="BV28" s="10"/>
-      <c r="CA28" s="10"/>
+      <c r="BS28" s="8"/>
+      <c r="BT28" s="8"/>
+      <c r="BV28" s="8"/>
+      <c r="CA28" s="8"/>
     </row>
     <row r="29" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -4712,35 +4672,34 @@
       <c r="AR29" t="s">
         <v>519</v>
       </c>
-      <c r="AS29" s="11" t="s">
+      <c r="AS29" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ29" s="1">
         <v>20</v>
       </c>
-      <c r="BA29" s="4" t="s">
+      <c r="BA29" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="BB29" s="11" t="s">
+      <c r="BB29" s="9" t="s">
         <v>267</v>
       </c>
       <c r="BD29" s="1">
         <v>20</v>
       </c>
-      <c r="BE29" s="4" t="s">
+      <c r="BE29" s="3" t="s">
         <v>352</v>
       </c>
       <c r="BP29" s="1">
         <v>20</v>
       </c>
-      <c r="BR29" s="10" t="s">
+      <c r="BR29" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="BS29" s="10"/>
-      <c r="BT29" s="10"/>
-      <c r="BU29" s="13"/>
-      <c r="BV29" s="10"/>
-      <c r="CA29" s="10"/>
+      <c r="BS29" s="8"/>
+      <c r="BT29" s="8"/>
+      <c r="BV29" s="8"/>
+      <c r="CA29" s="8"/>
     </row>
     <row r="30" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -4785,29 +4744,28 @@
       <c r="AR30" t="s">
         <v>520</v>
       </c>
-      <c r="AS30" s="11" t="s">
+      <c r="AS30" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ30" s="1">
         <v>21</v>
       </c>
-      <c r="BA30" s="8" t="s">
+      <c r="BA30" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="BB30" s="11" t="s">
+      <c r="BB30" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP30" s="1">
         <v>21</v>
       </c>
-      <c r="BR30" s="10" t="s">
+      <c r="BR30" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="BS30" s="10"/>
-      <c r="BT30" s="10"/>
-      <c r="BU30" s="13"/>
-      <c r="BV30" s="10"/>
-      <c r="CA30" s="10"/>
+      <c r="BS30" s="8"/>
+      <c r="BT30" s="8"/>
+      <c r="BV30" s="8"/>
+      <c r="CA30" s="8"/>
     </row>
     <row r="31" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -4852,29 +4810,28 @@
       <c r="AR31" t="s">
         <v>521</v>
       </c>
-      <c r="AS31" s="11" t="s">
+      <c r="AS31" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ31" s="1">
         <v>22</v>
       </c>
-      <c r="BA31" s="8" t="s">
+      <c r="BA31" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="BB31" s="11" t="s">
+      <c r="BB31" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP31" s="1">
         <v>22</v>
       </c>
-      <c r="BR31" s="10" t="s">
+      <c r="BR31" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="BS31" s="10"/>
-      <c r="BT31" s="10"/>
-      <c r="BU31" s="13"/>
-      <c r="BV31" s="10"/>
-      <c r="CA31" s="10"/>
+      <c r="BS31" s="8"/>
+      <c r="BT31" s="8"/>
+      <c r="BV31" s="8"/>
+      <c r="CA31" s="8"/>
     </row>
     <row r="32" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -4916,29 +4873,28 @@
       <c r="AR32" t="s">
         <v>522</v>
       </c>
-      <c r="AS32" s="11" t="s">
+      <c r="AS32" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ32" s="1">
         <v>23</v>
       </c>
-      <c r="BA32" s="8" t="s">
+      <c r="BA32" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="BB32" s="11" t="s">
+      <c r="BB32" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP32" s="1">
         <v>23</v>
       </c>
-      <c r="BR32" s="10" t="s">
+      <c r="BR32" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="BS32" s="10"/>
-      <c r="BT32" s="10"/>
-      <c r="BU32" s="13"/>
-      <c r="BV32" s="10"/>
-      <c r="CA32" s="10"/>
+      <c r="BS32" s="8"/>
+      <c r="BT32" s="8"/>
+      <c r="BV32" s="8"/>
+      <c r="CA32" s="8"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -4980,29 +4936,28 @@
       <c r="AR33" t="s">
         <v>523</v>
       </c>
-      <c r="AS33" s="11" t="s">
+      <c r="AS33" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ33" s="1">
         <v>24</v>
       </c>
-      <c r="BA33" s="8" t="s">
+      <c r="BA33" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="BB33" s="11" t="s">
+      <c r="BB33" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP33" s="1">
         <v>24</v>
       </c>
-      <c r="BR33" s="10" t="s">
+      <c r="BR33" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="BS33" s="10"/>
-      <c r="BT33" s="10"/>
-      <c r="BU33" s="13"/>
-      <c r="BV33" s="10"/>
-      <c r="CA33" s="10"/>
+      <c r="BS33" s="8"/>
+      <c r="BT33" s="8"/>
+      <c r="BV33" s="8"/>
+      <c r="CA33" s="8"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -5044,29 +4999,28 @@
       <c r="AR34" t="s">
         <v>524</v>
       </c>
-      <c r="AS34" s="11" t="s">
+      <c r="AS34" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ34" s="1">
         <v>25</v>
       </c>
-      <c r="BA34" s="8" t="s">
+      <c r="BA34" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="BB34" s="11" t="s">
+      <c r="BB34" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP34" s="1">
         <v>25</v>
       </c>
-      <c r="BR34" s="10" t="s">
+      <c r="BR34" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="BS34" s="10"/>
-      <c r="BT34" s="10"/>
-      <c r="BU34" s="13"/>
-      <c r="BV34" s="10"/>
-      <c r="CA34" s="10"/>
+      <c r="BS34" s="8"/>
+      <c r="BT34" s="8"/>
+      <c r="BV34" s="8"/>
+      <c r="CA34" s="8"/>
     </row>
     <row r="35" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -5108,22 +5062,21 @@
       <c r="AR35" t="s">
         <v>525</v>
       </c>
-      <c r="AS35" s="11" t="s">
+      <c r="AS35" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ35" s="1">
         <v>26</v>
       </c>
-      <c r="BA35" s="8" t="s">
+      <c r="BA35" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="BB35" s="11" t="s">
+      <c r="BB35" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP35" s="1">
         <v>26</v>
       </c>
-      <c r="BU35" s="13"/>
     </row>
     <row r="36" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -5165,16 +5118,16 @@
       <c r="AR36" t="s">
         <v>526</v>
       </c>
-      <c r="AS36" s="11" t="s">
+      <c r="AS36" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ36" s="1">
         <v>27</v>
       </c>
-      <c r="BA36" s="4" t="s">
+      <c r="BA36" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="BB36" s="11" t="s">
+      <c r="BB36" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP36" s="1">
@@ -5221,16 +5174,16 @@
       <c r="AR37" t="s">
         <v>527</v>
       </c>
-      <c r="AS37" s="11" t="s">
+      <c r="AS37" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ37" s="1">
         <v>28</v>
       </c>
-      <c r="BA37" s="4" t="s">
+      <c r="BA37" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="BB37" s="11" t="s">
+      <c r="BB37" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP37" s="1" t="s">
@@ -5277,16 +5230,16 @@
       <c r="AR38" t="s">
         <v>528</v>
       </c>
-      <c r="AS38" s="11" t="s">
+      <c r="AS38" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ38" s="1">
         <v>29</v>
       </c>
-      <c r="BA38" s="4" t="s">
+      <c r="BA38" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="BB38" s="11" t="s">
+      <c r="BB38" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP38" s="1" t="s">
@@ -5333,16 +5286,16 @@
       <c r="AR39" t="s">
         <v>529</v>
       </c>
-      <c r="AS39" s="11" t="s">
+      <c r="AS39" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ39" s="1">
         <v>30</v>
       </c>
-      <c r="BA39" s="4" t="s">
+      <c r="BA39" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="BB39" s="11" t="s">
+      <c r="BB39" s="9" t="s">
         <v>317</v>
       </c>
       <c r="BP39" s="1" t="s">
@@ -5383,16 +5336,16 @@
       <c r="AR40" t="s">
         <v>530</v>
       </c>
-      <c r="AS40" s="11" t="s">
+      <c r="AS40" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ40" s="1">
         <v>31</v>
       </c>
-      <c r="BA40" s="4" t="s">
+      <c r="BA40" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="BB40" s="11" t="s">
+      <c r="BB40" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5430,16 +5383,16 @@
       <c r="AR41" t="s">
         <v>531</v>
       </c>
-      <c r="AS41" s="11" t="s">
+      <c r="AS41" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ41" s="1">
         <v>32</v>
       </c>
-      <c r="BA41" s="4" t="s">
+      <c r="BA41" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="BB41" s="11" t="s">
+      <c r="BB41" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5477,16 +5430,16 @@
       <c r="AR42" t="s">
         <v>532</v>
       </c>
-      <c r="AS42" s="11" t="s">
+      <c r="AS42" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ42" s="1">
         <v>33</v>
       </c>
-      <c r="BA42" s="4" t="s">
+      <c r="BA42" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="BB42" s="11" t="s">
+      <c r="BB42" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5524,16 +5477,16 @@
       <c r="AR43" t="s">
         <v>533</v>
       </c>
-      <c r="AS43" s="11" t="s">
+      <c r="AS43" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ43" s="1">
         <v>34</v>
       </c>
-      <c r="BA43" s="4" t="s">
+      <c r="BA43" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="BB43" s="11" t="s">
+      <c r="BB43" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5571,16 +5524,16 @@
       <c r="AR44" t="s">
         <v>534</v>
       </c>
-      <c r="AS44" s="11" t="s">
+      <c r="AS44" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ44" s="1">
         <v>35</v>
       </c>
-      <c r="BA44" s="4" t="s">
+      <c r="BA44" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="BB44" s="11" t="s">
+      <c r="BB44" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5618,16 +5571,16 @@
       <c r="AR45" t="s">
         <v>535</v>
       </c>
-      <c r="AS45" s="11" t="s">
+      <c r="AS45" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ45" s="1">
         <v>36</v>
       </c>
-      <c r="BA45" s="4" t="s">
+      <c r="BA45" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="BB45" s="11" t="s">
+      <c r="BB45" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5665,16 +5618,16 @@
       <c r="AR46" t="s">
         <v>528</v>
       </c>
-      <c r="AS46" s="11" t="s">
+      <c r="AS46" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ46" s="1">
         <v>37</v>
       </c>
-      <c r="BA46" s="8" t="s">
+      <c r="BA46" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="BB46" s="11" t="s">
+      <c r="BB46" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5712,16 +5665,16 @@
       <c r="AR47" t="s">
         <v>536</v>
       </c>
-      <c r="AS47" s="11" t="s">
+      <c r="AS47" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ47" s="1">
         <v>38</v>
       </c>
-      <c r="BA47" s="8" t="s">
+      <c r="BA47" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="BB47" s="11" t="s">
+      <c r="BB47" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5759,16 +5712,16 @@
       <c r="AR48" t="s">
         <v>537</v>
       </c>
-      <c r="AS48" s="11" t="s">
+      <c r="AS48" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ48" s="1">
         <v>39</v>
       </c>
-      <c r="BA48" s="8" t="s">
+      <c r="BA48" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="BB48" s="11" t="s">
+      <c r="BB48" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5806,16 +5759,16 @@
       <c r="AR49" t="s">
         <v>538</v>
       </c>
-      <c r="AS49" s="11" t="s">
+      <c r="AS49" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ49" s="1">
         <v>40</v>
       </c>
-      <c r="BA49" s="8" t="s">
+      <c r="BA49" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="BB49" s="11" t="s">
+      <c r="BB49" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5853,16 +5806,16 @@
       <c r="AR50" t="s">
         <v>539</v>
       </c>
-      <c r="AS50" s="11" t="s">
+      <c r="AS50" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ50" s="1">
         <v>41</v>
       </c>
-      <c r="BA50" s="8" t="s">
+      <c r="BA50" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="BB50" s="11" t="s">
+      <c r="BB50" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5900,16 +5853,16 @@
       <c r="AR51" t="s">
         <v>540</v>
       </c>
-      <c r="AS51" s="11" t="s">
+      <c r="AS51" s="9" t="s">
         <v>475</v>
       </c>
       <c r="AZ51" s="1">
         <v>42</v>
       </c>
-      <c r="BA51" s="8" t="s">
+      <c r="BA51" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="BB51" s="11" t="s">
+      <c r="BB51" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5947,16 +5900,16 @@
       <c r="AR52" t="s">
         <v>500</v>
       </c>
-      <c r="AS52" s="10" t="s">
+      <c r="AS52" s="8" t="s">
         <v>500</v>
       </c>
       <c r="AZ52" s="1">
         <v>43</v>
       </c>
-      <c r="BA52" s="8" t="s">
+      <c r="BA52" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="BB52" s="11" t="s">
+      <c r="BB52" s="9" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5994,16 +5947,16 @@
       <c r="AR53" t="s">
         <v>541</v>
       </c>
-      <c r="AS53" s="11" t="s">
+      <c r="AS53" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ53" s="1">
         <v>44</v>
       </c>
-      <c r="BA53" s="4" t="s">
+      <c r="BA53" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="BB53" s="11" t="s">
+      <c r="BB53" s="9" t="s">
         <v>318</v>
       </c>
     </row>
@@ -6041,16 +5994,16 @@
       <c r="AR54" t="s">
         <v>542</v>
       </c>
-      <c r="AS54" s="11" t="s">
+      <c r="AS54" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ54" s="1">
         <v>45</v>
       </c>
-      <c r="BA54" s="4" t="s">
+      <c r="BA54" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="BB54" s="11" t="s">
+      <c r="BB54" s="9" t="s">
         <v>318</v>
       </c>
     </row>
@@ -6088,16 +6041,16 @@
       <c r="AR55" t="s">
         <v>543</v>
       </c>
-      <c r="AS55" s="11" t="s">
+      <c r="AS55" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ55" s="1">
         <v>46</v>
       </c>
-      <c r="BA55" s="4" t="s">
+      <c r="BA55" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="BB55" s="11" t="s">
+      <c r="BB55" s="9" t="s">
         <v>318</v>
       </c>
     </row>
@@ -6135,16 +6088,16 @@
       <c r="AR56" t="s">
         <v>544</v>
       </c>
-      <c r="AS56" s="11" t="s">
+      <c r="AS56" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ56" s="1">
         <v>47</v>
       </c>
-      <c r="BA56" s="4" t="s">
+      <c r="BA56" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="BB56" s="11" t="s">
+      <c r="BB56" s="9" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6182,16 +6135,16 @@
       <c r="AR57" t="s">
         <v>545</v>
       </c>
-      <c r="AS57" s="11" t="s">
+      <c r="AS57" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ57" s="1">
         <v>48</v>
       </c>
-      <c r="BA57" s="4" t="s">
+      <c r="BA57" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="BB57" s="11" t="s">
+      <c r="BB57" s="9" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6229,16 +6182,16 @@
       <c r="AR58" t="s">
         <v>546</v>
       </c>
-      <c r="AS58" s="11" t="s">
+      <c r="AS58" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ58" s="1">
         <v>49</v>
       </c>
-      <c r="BA58" s="4" t="s">
+      <c r="BA58" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="BB58" s="11" t="s">
+      <c r="BB58" s="9" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6276,16 +6229,16 @@
       <c r="AR59" t="s">
         <v>547</v>
       </c>
-      <c r="AS59" s="11" t="s">
+      <c r="AS59" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ59" s="1">
         <v>50</v>
       </c>
-      <c r="BA59" s="4" t="s">
+      <c r="BA59" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="BB59" s="11" t="s">
+      <c r="BB59" s="9" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6323,16 +6276,16 @@
       <c r="AR60" t="s">
         <v>548</v>
       </c>
-      <c r="AS60" s="11" t="s">
+      <c r="AS60" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ60" s="1">
         <v>51</v>
       </c>
-      <c r="BA60" s="4" t="s">
+      <c r="BA60" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="BB60" s="11" t="s">
+      <c r="BB60" s="9" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6370,16 +6323,16 @@
       <c r="AR61" t="s">
         <v>549</v>
       </c>
-      <c r="AS61" s="11" t="s">
+      <c r="AS61" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ61" s="1">
         <v>52</v>
       </c>
-      <c r="BA61" s="4" t="s">
+      <c r="BA61" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="BB61" s="11" t="s">
+      <c r="BB61" s="9" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6417,16 +6370,16 @@
       <c r="AR62" t="s">
         <v>550</v>
       </c>
-      <c r="AS62" s="11" t="s">
+      <c r="AS62" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ62" s="1">
         <v>53</v>
       </c>
-      <c r="BA62" s="4" t="s">
+      <c r="BA62" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="BB62" s="11" t="s">
+      <c r="BB62" s="9" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6464,16 +6417,16 @@
       <c r="AR63" t="s">
         <v>551</v>
       </c>
-      <c r="AS63" s="11" t="s">
+      <c r="AS63" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ63" s="1">
         <v>54</v>
       </c>
-      <c r="BA63" s="4" t="s">
+      <c r="BA63" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="BB63" s="11" t="s">
+      <c r="BB63" s="9" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6511,16 +6464,16 @@
       <c r="AR64" t="s">
         <v>552</v>
       </c>
-      <c r="AS64" s="11" t="s">
+      <c r="AS64" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ64" s="1">
         <v>55</v>
       </c>
-      <c r="BA64" s="4" t="s">
+      <c r="BA64" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="BB64" s="11" t="s">
+      <c r="BB64" s="9" t="s">
         <v>313</v>
       </c>
     </row>
@@ -6558,16 +6511,16 @@
       <c r="AR65" t="s">
         <v>553</v>
       </c>
-      <c r="AS65" s="11" t="s">
+      <c r="AS65" s="9" t="s">
         <v>244</v>
       </c>
       <c r="AZ65" s="1">
         <v>56</v>
       </c>
-      <c r="BA65" s="4" t="s">
+      <c r="BA65" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="BB65" s="11" t="s">
+      <c r="BB65" s="9" t="s">
         <v>313</v>
       </c>
     </row>
@@ -6605,16 +6558,16 @@
       <c r="AR66" t="s">
         <v>554</v>
       </c>
-      <c r="AS66" s="10" t="s">
+      <c r="AS66" s="8" t="s">
         <v>476</v>
       </c>
       <c r="AZ66" s="1">
         <v>57</v>
       </c>
-      <c r="BA66" s="4" t="s">
+      <c r="BA66" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="BB66" s="11" t="s">
+      <c r="BB66" s="9" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6652,16 +6605,16 @@
       <c r="AR67" t="s">
         <v>555</v>
       </c>
-      <c r="AS67" s="10" t="s">
+      <c r="AS67" s="8" t="s">
         <v>476</v>
       </c>
       <c r="AZ67" s="1">
         <v>58</v>
       </c>
-      <c r="BA67" s="4" t="s">
+      <c r="BA67" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="BB67" s="11" t="s">
+      <c r="BB67" s="9" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6699,16 +6652,16 @@
       <c r="AR68" t="s">
         <v>556</v>
       </c>
-      <c r="AS68" s="10" t="s">
+      <c r="AS68" s="8" t="s">
         <v>476</v>
       </c>
       <c r="AZ68" s="1">
         <v>59</v>
       </c>
-      <c r="BA68" s="4" t="s">
+      <c r="BA68" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="BB68" s="11" t="s">
+      <c r="BB68" s="9" t="s">
         <v>313</v>
       </c>
     </row>
@@ -6746,16 +6699,16 @@
       <c r="AR69" t="s">
         <v>557</v>
       </c>
-      <c r="AS69" s="10" t="s">
+      <c r="AS69" s="8" t="s">
         <v>476</v>
       </c>
       <c r="AZ69" s="1">
         <v>60</v>
       </c>
-      <c r="BA69" s="4" t="s">
+      <c r="BA69" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="BB69" s="11" t="s">
+      <c r="BB69" s="9" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6793,16 +6746,16 @@
       <c r="AR70" t="s">
         <v>558</v>
       </c>
-      <c r="AS70" s="10" t="s">
+      <c r="AS70" s="8" t="s">
         <v>476</v>
       </c>
       <c r="AZ70" s="1">
         <v>61</v>
       </c>
-      <c r="BA70" s="4" t="s">
+      <c r="BA70" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="BB70" s="11" t="s">
+      <c r="BB70" s="9" t="s">
         <v>313</v>
       </c>
     </row>
@@ -6840,16 +6793,16 @@
       <c r="AR71" t="s">
         <v>559</v>
       </c>
-      <c r="AS71" s="10" t="s">
+      <c r="AS71" s="8" t="s">
         <v>476</v>
       </c>
       <c r="AZ71" s="1">
         <v>62</v>
       </c>
-      <c r="BA71" s="4" t="s">
+      <c r="BA71" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="BB71" s="11" t="s">
+      <c r="BB71" s="9" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6884,19 +6837,19 @@
       <c r="AQ72" s="1">
         <v>63</v>
       </c>
-      <c r="AR72" s="9" t="s">
+      <c r="AR72" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="AS72" s="10" t="s">
+      <c r="AS72" s="8" t="s">
         <v>476</v>
       </c>
       <c r="AZ72" s="1">
         <v>63</v>
       </c>
-      <c r="BA72" s="4" t="s">
+      <c r="BA72" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="BB72" s="11" t="s">
+      <c r="BB72" s="9" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6931,19 +6884,19 @@
       <c r="AQ73" s="1">
         <v>64</v>
       </c>
-      <c r="AR73" s="9" t="s">
+      <c r="AR73" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="AS73" s="10" t="s">
+      <c r="AS73" s="8" t="s">
         <v>476</v>
       </c>
       <c r="AZ73" s="1">
         <v>64</v>
       </c>
-      <c r="BA73" s="4" t="s">
+      <c r="BA73" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="BB73" s="11" t="s">
+      <c r="BB73" s="9" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6978,19 +6931,19 @@
       <c r="AQ74" s="1">
         <v>65</v>
       </c>
-      <c r="AR74" s="4" t="s">
+      <c r="AR74" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="AS74" s="11" t="s">
+      <c r="AS74" s="9" t="s">
         <v>477</v>
       </c>
       <c r="AZ74" s="1">
         <v>65</v>
       </c>
-      <c r="BA74" s="4" t="s">
+      <c r="BA74" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="BB74" s="11" t="s">
+      <c r="BB74" s="9" t="s">
         <v>312</v>
       </c>
     </row>
@@ -7025,19 +6978,19 @@
       <c r="AQ75" s="1">
         <v>66</v>
       </c>
-      <c r="AR75" s="4" t="s">
+      <c r="AR75" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="AS75" s="11" t="s">
+      <c r="AS75" s="9" t="s">
         <v>478</v>
       </c>
       <c r="AZ75" s="1">
         <v>66</v>
       </c>
-      <c r="BA75" s="4" t="s">
+      <c r="BA75" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="BB75" s="11" t="s">
+      <c r="BB75" s="9" t="s">
         <v>313</v>
       </c>
     </row>
@@ -7072,19 +7025,19 @@
       <c r="AQ76" s="1">
         <v>67</v>
       </c>
-      <c r="AR76" s="4" t="s">
+      <c r="AR76" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="AS76" s="11" t="s">
+      <c r="AS76" s="9" t="s">
         <v>479</v>
       </c>
       <c r="AZ76" s="1">
         <v>67</v>
       </c>
-      <c r="BA76" s="9" t="s">
+      <c r="BA76" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="BB76" s="12" t="s">
+      <c r="BB76" s="10" t="s">
         <v>314</v>
       </c>
     </row>
@@ -7119,19 +7072,19 @@
       <c r="AQ77" s="1">
         <v>68</v>
       </c>
-      <c r="AR77" s="4" t="s">
+      <c r="AR77" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="AS77" s="11" t="s">
+      <c r="AS77" s="9" t="s">
         <v>479</v>
       </c>
       <c r="AZ77" s="1">
         <v>68</v>
       </c>
-      <c r="BA77" s="9" t="s">
+      <c r="BA77" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="BB77" s="12" t="s">
+      <c r="BB77" s="10" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7166,19 +7119,19 @@
       <c r="AQ78" s="1">
         <v>69</v>
       </c>
-      <c r="AR78" s="4" t="s">
+      <c r="AR78" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="AS78" s="11" t="s">
+      <c r="AS78" s="9" t="s">
         <v>498</v>
       </c>
       <c r="AZ78" s="1">
         <v>69</v>
       </c>
-      <c r="BA78" s="9" t="s">
+      <c r="BA78" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="BB78" s="12" t="s">
+      <c r="BB78" s="10" t="s">
         <v>344</v>
       </c>
     </row>
@@ -7216,16 +7169,16 @@
       <c r="AR79" t="s">
         <v>485</v>
       </c>
-      <c r="AS79" s="11" t="s">
+      <c r="AS79" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ79" s="1">
         <v>70</v>
       </c>
-      <c r="BA79" s="9" t="s">
+      <c r="BA79" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="BB79" s="12" t="s">
+      <c r="BB79" s="10" t="s">
         <v>344</v>
       </c>
     </row>
@@ -7263,16 +7216,16 @@
       <c r="AR80" t="s">
         <v>486</v>
       </c>
-      <c r="AS80" s="11" t="s">
+      <c r="AS80" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ80" s="1">
         <v>71</v>
       </c>
-      <c r="BA80" s="9" t="s">
+      <c r="BA80" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="BB80" s="12" t="s">
+      <c r="BB80" s="10" t="s">
         <v>344</v>
       </c>
     </row>
@@ -7310,16 +7263,16 @@
       <c r="AR81" t="s">
         <v>487</v>
       </c>
-      <c r="AS81" s="11" t="s">
+      <c r="AS81" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ81" s="1">
         <v>72</v>
       </c>
-      <c r="BA81" s="9" t="s">
+      <c r="BA81" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="BB81" s="12" t="s">
+      <c r="BB81" s="10" t="s">
         <v>344</v>
       </c>
     </row>
@@ -7357,16 +7310,16 @@
       <c r="AR82" t="s">
         <v>488</v>
       </c>
-      <c r="AS82" s="11" t="s">
+      <c r="AS82" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ82" s="1">
         <v>73</v>
       </c>
-      <c r="BA82" s="9" t="s">
+      <c r="BA82" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="BB82" s="12" t="s">
+      <c r="BB82" s="10" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7404,16 +7357,16 @@
       <c r="AR83" t="s">
         <v>489</v>
       </c>
-      <c r="AS83" s="11" t="s">
+      <c r="AS83" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ83" s="1">
         <v>74</v>
       </c>
-      <c r="BA83" s="9" t="s">
+      <c r="BA83" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="BB83" s="12" t="s">
+      <c r="BB83" s="10" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7451,16 +7404,16 @@
       <c r="AR84" t="s">
         <v>490</v>
       </c>
-      <c r="AS84" s="11" t="s">
+      <c r="AS84" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ84" s="1">
         <v>75</v>
       </c>
-      <c r="BA84" s="9" t="s">
+      <c r="BA84" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="BB84" s="12" t="s">
+      <c r="BB84" s="10" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7498,16 +7451,16 @@
       <c r="AR85" t="s">
         <v>491</v>
       </c>
-      <c r="AS85" s="11" t="s">
+      <c r="AS85" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ85" s="1">
         <v>76</v>
       </c>
-      <c r="BA85" s="9" t="s">
+      <c r="BA85" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="BB85" s="12" t="s">
+      <c r="BB85" s="10" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7545,16 +7498,16 @@
       <c r="AR86" t="s">
         <v>492</v>
       </c>
-      <c r="AS86" s="11" t="s">
+      <c r="AS86" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ86" s="1">
         <v>77</v>
       </c>
-      <c r="BA86" s="9" t="s">
+      <c r="BA86" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="BB86" s="12" t="s">
+      <c r="BB86" s="10" t="s">
         <v>323</v>
       </c>
     </row>
@@ -7592,16 +7545,16 @@
       <c r="AR87" t="s">
         <v>493</v>
       </c>
-      <c r="AS87" s="11" t="s">
+      <c r="AS87" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ87" s="1">
         <v>78</v>
       </c>
-      <c r="BA87" s="9" t="s">
+      <c r="BA87" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="BB87" s="12" t="s">
+      <c r="BB87" s="10" t="s">
         <v>323</v>
       </c>
     </row>
@@ -7639,20 +7592,20 @@
       <c r="AR88" t="s">
         <v>494</v>
       </c>
-      <c r="AS88" s="11" t="s">
+      <c r="AS88" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ88" s="1">
         <v>79</v>
       </c>
-      <c r="BA88" s="9" t="s">
+      <c r="BA88" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="BB88" s="12" t="s">
+      <c r="BB88" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="BP88" s="9"/>
-      <c r="BQ88" s="9"/>
+      <c r="BP88" s="7"/>
+      <c r="BQ88" s="7"/>
     </row>
     <row r="89" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
@@ -7688,30 +7641,30 @@
       <c r="AR89" t="s">
         <v>495</v>
       </c>
-      <c r="AS89" s="11" t="s">
+      <c r="AS89" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ89" s="1">
         <v>80</v>
       </c>
-      <c r="BA89" s="9" t="s">
+      <c r="BA89" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="BB89" s="12" t="s">
+      <c r="BB89" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="BF89" s="9"/>
-      <c r="BG89" s="9"/>
-      <c r="BH89" s="9"/>
-      <c r="BI89" s="9"/>
-      <c r="BJ89" s="9"/>
-      <c r="BK89" s="9"/>
-      <c r="BL89" s="9"/>
-      <c r="BM89" s="9"/>
-      <c r="BN89" s="9"/>
-      <c r="BO89" s="9"/>
-      <c r="BP89" s="9"/>
-      <c r="BQ89" s="9"/>
+      <c r="BF89" s="7"/>
+      <c r="BG89" s="7"/>
+      <c r="BH89" s="7"/>
+      <c r="BI89" s="7"/>
+      <c r="BJ89" s="7"/>
+      <c r="BK89" s="7"/>
+      <c r="BL89" s="7"/>
+      <c r="BM89" s="7"/>
+      <c r="BN89" s="7"/>
+      <c r="BO89" s="7"/>
+      <c r="BP89" s="7"/>
+      <c r="BQ89" s="7"/>
     </row>
     <row r="90" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -7747,30 +7700,30 @@
       <c r="AR90" t="s">
         <v>496</v>
       </c>
-      <c r="AS90" s="11" t="s">
+      <c r="AS90" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ90" s="1">
         <v>81</v>
       </c>
-      <c r="BA90" s="9" t="s">
+      <c r="BA90" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="BB90" s="12" t="s">
+      <c r="BB90" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="BF90" s="9"/>
-      <c r="BG90" s="9"/>
-      <c r="BH90" s="9"/>
-      <c r="BI90" s="9"/>
-      <c r="BJ90" s="9"/>
-      <c r="BK90" s="9"/>
-      <c r="BL90" s="9"/>
-      <c r="BM90" s="9"/>
-      <c r="BN90" s="9"/>
-      <c r="BO90" s="9"/>
-      <c r="BP90" s="9"/>
-      <c r="BQ90" s="9"/>
+      <c r="BF90" s="7"/>
+      <c r="BG90" s="7"/>
+      <c r="BH90" s="7"/>
+      <c r="BI90" s="7"/>
+      <c r="BJ90" s="7"/>
+      <c r="BK90" s="7"/>
+      <c r="BL90" s="7"/>
+      <c r="BM90" s="7"/>
+      <c r="BN90" s="7"/>
+      <c r="BO90" s="7"/>
+      <c r="BP90" s="7"/>
+      <c r="BQ90" s="7"/>
     </row>
     <row r="91" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
@@ -7806,16 +7759,16 @@
       <c r="AR91" t="s">
         <v>497</v>
       </c>
-      <c r="AS91" s="11" t="s">
+      <c r="AS91" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ91" s="1">
         <v>82</v>
       </c>
-      <c r="BA91" s="9" t="s">
+      <c r="BA91" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="BB91" s="12" t="s">
+      <c r="BB91" s="10" t="s">
         <v>327</v>
       </c>
     </row>
@@ -7853,16 +7806,16 @@
       <c r="AR92" t="s">
         <v>491</v>
       </c>
-      <c r="AS92" s="11" t="s">
+      <c r="AS92" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ92" s="1">
         <v>83</v>
       </c>
-      <c r="BA92" s="9" t="s">
+      <c r="BA92" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="BB92" s="12" t="s">
+      <c r="BB92" s="10" t="s">
         <v>327</v>
       </c>
     </row>
@@ -7900,16 +7853,16 @@
       <c r="AR93" t="s">
         <v>484</v>
       </c>
-      <c r="AS93" s="11" t="s">
+      <c r="AS93" s="9" t="s">
         <v>499</v>
       </c>
       <c r="AZ93" s="1">
         <v>84</v>
       </c>
-      <c r="BA93" s="9" t="s">
+      <c r="BA93" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="BB93" s="12" t="s">
+      <c r="BB93" s="10" t="s">
         <v>327</v>
       </c>
     </row>
@@ -7947,16 +7900,16 @@
       <c r="AR94" t="s">
         <v>380</v>
       </c>
-      <c r="AS94" s="11" t="s">
+      <c r="AS94" s="9" t="s">
         <v>380</v>
       </c>
       <c r="AZ94" s="1">
         <v>85</v>
       </c>
-      <c r="BA94" s="9" t="s">
+      <c r="BA94" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="BB94" s="12" t="s">
+      <c r="BB94" s="10" t="s">
         <v>327</v>
       </c>
     </row>
@@ -7994,14 +7947,14 @@
       <c r="AR95" t="s">
         <v>390</v>
       </c>
-      <c r="AS95" s="10"/>
+      <c r="AS95" s="8"/>
       <c r="AZ95" s="1">
         <v>86</v>
       </c>
-      <c r="BA95" s="9" t="s">
+      <c r="BA95" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="BB95" s="12" t="s">
+      <c r="BB95" s="10" t="s">
         <v>327</v>
       </c>
     </row>
@@ -8039,14 +7992,14 @@
       <c r="AR96" t="s">
         <v>391</v>
       </c>
-      <c r="AS96" s="10"/>
+      <c r="AS96" s="8"/>
       <c r="AZ96" s="1">
         <v>87</v>
       </c>
-      <c r="BA96" s="9" t="s">
+      <c r="BA96" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="BB96" s="12" t="s">
+      <c r="BB96" s="10" t="s">
         <v>349</v>
       </c>
     </row>
@@ -8084,14 +8037,14 @@
       <c r="AR97" t="s">
         <v>392</v>
       </c>
-      <c r="AS97" s="10"/>
+      <c r="AS97" s="8"/>
       <c r="AZ97" s="1">
         <v>88</v>
       </c>
-      <c r="BA97" s="9" t="s">
+      <c r="BA97" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="BB97" s="12" t="s">
+      <c r="BB97" s="10" t="s">
         <v>349</v>
       </c>
     </row>
@@ -8129,14 +8082,14 @@
       <c r="AR98" t="s">
         <v>393</v>
       </c>
-      <c r="AS98" s="10"/>
+      <c r="AS98" s="8"/>
       <c r="AZ98" s="1">
         <v>89</v>
       </c>
-      <c r="BA98" s="9" t="s">
+      <c r="BA98" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="BB98" s="12" t="s">
+      <c r="BB98" s="10" t="s">
         <v>349</v>
       </c>
     </row>
@@ -8174,14 +8127,14 @@
       <c r="AR99" t="s">
         <v>394</v>
       </c>
-      <c r="AS99" s="10"/>
+      <c r="AS99" s="8"/>
       <c r="AZ99" s="1">
         <v>90</v>
       </c>
-      <c r="BA99" s="9" t="s">
+      <c r="BA99" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="BB99" s="12" t="s">
+      <c r="BB99" s="10" t="s">
         <v>340</v>
       </c>
     </row>
@@ -8219,14 +8172,14 @@
       <c r="AR100" t="s">
         <v>395</v>
       </c>
-      <c r="AS100" s="10"/>
+      <c r="AS100" s="8"/>
       <c r="AZ100" s="1">
         <v>91</v>
       </c>
-      <c r="BA100" s="9" t="s">
+      <c r="BA100" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="BB100" s="12" t="s">
+      <c r="BB100" s="10" t="s">
         <v>340</v>
       </c>
     </row>
@@ -8264,14 +8217,14 @@
       <c r="AR101" t="s">
         <v>396</v>
       </c>
-      <c r="AS101" s="10"/>
+      <c r="AS101" s="8"/>
       <c r="AZ101" s="1">
         <v>92</v>
       </c>
-      <c r="BA101" s="9" t="s">
+      <c r="BA101" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="BB101" s="12" t="s">
+      <c r="BB101" s="10" t="s">
         <v>340</v>
       </c>
     </row>
@@ -8309,14 +8262,14 @@
       <c r="AR102" t="s">
         <v>397</v>
       </c>
-      <c r="AS102" s="10"/>
+      <c r="AS102" s="8"/>
       <c r="AZ102" s="1">
         <v>93</v>
       </c>
-      <c r="BA102" s="9" t="s">
+      <c r="BA102" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="BB102" s="12" t="s">
+      <c r="BB102" s="10" t="s">
         <v>337</v>
       </c>
     </row>
@@ -8354,17 +8307,17 @@
       <c r="AR103" t="s">
         <v>398</v>
       </c>
-      <c r="AS103" s="10"/>
+      <c r="AS103" s="8"/>
       <c r="AZ103" s="1">
         <v>94</v>
       </c>
-      <c r="BA103" s="9" t="s">
+      <c r="BA103" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="BB103" s="12" t="s">
+      <c r="BB103" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="BE103" s="9"/>
+      <c r="BE103" s="7"/>
     </row>
     <row r="104" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
@@ -8400,14 +8353,14 @@
       <c r="AR104" t="s">
         <v>399</v>
       </c>
-      <c r="AS104" s="10"/>
+      <c r="AS104" s="8"/>
       <c r="AZ104" s="1">
         <v>95</v>
       </c>
-      <c r="BA104" s="9" t="s">
+      <c r="BA104" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="BB104" s="12" t="s">
+      <c r="BB104" s="10" t="s">
         <v>334</v>
       </c>
     </row>
@@ -8445,14 +8398,14 @@
       <c r="AR105" t="s">
         <v>400</v>
       </c>
-      <c r="AS105" s="10"/>
+      <c r="AS105" s="8"/>
       <c r="AZ105" s="1">
         <v>96</v>
       </c>
-      <c r="BA105" s="9" t="s">
+      <c r="BA105" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="BB105" s="12" t="s">
+      <c r="BB105" s="10" t="s">
         <v>335</v>
       </c>
     </row>
@@ -8490,14 +8443,14 @@
       <c r="AR106" t="s">
         <v>401</v>
       </c>
-      <c r="AS106" s="10"/>
+      <c r="AS106" s="8"/>
       <c r="AZ106" s="1">
         <v>97</v>
       </c>
-      <c r="BA106" s="9" t="s">
+      <c r="BA106" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="BB106" s="12" t="s">
+      <c r="BB106" s="10" t="s">
         <v>357</v>
       </c>
     </row>
@@ -8535,17 +8488,17 @@
       <c r="AR107" t="s">
         <v>402</v>
       </c>
-      <c r="AS107" s="10"/>
+      <c r="AS107" s="8"/>
       <c r="AZ107" s="1">
         <v>98</v>
       </c>
-      <c r="BA107" s="9" t="s">
+      <c r="BA107" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="BB107" s="12" t="s">
+      <c r="BB107" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="BE107" s="9"/>
+      <c r="BE107" s="7"/>
     </row>
     <row r="108" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
@@ -8581,17 +8534,17 @@
       <c r="AR108" t="s">
         <v>403</v>
       </c>
-      <c r="AS108" s="10"/>
+      <c r="AS108" s="8"/>
       <c r="AZ108" s="1">
         <v>99</v>
       </c>
-      <c r="BA108" s="9" t="s">
+      <c r="BA108" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="BB108" s="12" t="s">
+      <c r="BB108" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="BE108" s="9"/>
+      <c r="BE108" s="7"/>
     </row>
     <row r="109" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
@@ -8627,7 +8580,7 @@
       <c r="AR109" t="s">
         <v>404</v>
       </c>
-      <c r="AS109" s="10"/>
+      <c r="AS109" s="8"/>
     </row>
     <row r="110" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
@@ -8663,7 +8616,7 @@
       <c r="AR110" t="s">
         <v>405</v>
       </c>
-      <c r="AS110" s="10"/>
+      <c r="AS110" s="8"/>
     </row>
     <row r="111" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
@@ -8699,7 +8652,7 @@
       <c r="AR111" t="s">
         <v>406</v>
       </c>
-      <c r="AS111" s="10"/>
+      <c r="AS111" s="8"/>
     </row>
     <row r="112" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
@@ -8735,9 +8688,9 @@
       <c r="AR112" t="s">
         <v>407</v>
       </c>
-      <c r="AS112" s="10"/>
-      <c r="BA112" s="9"/>
-      <c r="BB112" s="9"/>
+      <c r="AS112" s="8"/>
+      <c r="BA112" s="7"/>
+      <c r="BB112" s="7"/>
     </row>
     <row r="113" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
@@ -8773,7 +8726,7 @@
       <c r="AR113" t="s">
         <v>408</v>
       </c>
-      <c r="AS113" s="10"/>
+      <c r="AS113" s="8"/>
     </row>
     <row r="114" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
@@ -8809,7 +8762,7 @@
       <c r="AR114" t="s">
         <v>409</v>
       </c>
-      <c r="AS114" s="10"/>
+      <c r="AS114" s="8"/>
     </row>
     <row r="115" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
@@ -8845,7 +8798,7 @@
       <c r="AR115" t="s">
         <v>410</v>
       </c>
-      <c r="AS115" s="10"/>
+      <c r="AS115" s="8"/>
     </row>
     <row r="116" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
@@ -8881,7 +8834,7 @@
       <c r="AR116" t="s">
         <v>411</v>
       </c>
-      <c r="AS116" s="10"/>
+      <c r="AS116" s="8"/>
     </row>
     <row r="117" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
@@ -8917,7 +8870,7 @@
       <c r="AR117" t="s">
         <v>412</v>
       </c>
-      <c r="AS117" s="10"/>
+      <c r="AS117" s="8"/>
     </row>
     <row r="118" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
@@ -8953,7 +8906,7 @@
       <c r="AR118" t="s">
         <v>413</v>
       </c>
-      <c r="AS118" s="10"/>
+      <c r="AS118" s="8"/>
     </row>
     <row r="119" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
@@ -8989,7 +8942,7 @@
       <c r="AR119" t="s">
         <v>414</v>
       </c>
-      <c r="AS119" s="10"/>
+      <c r="AS119" s="8"/>
     </row>
     <row r="120" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
@@ -9025,7 +8978,7 @@
       <c r="AR120" t="s">
         <v>415</v>
       </c>
-      <c r="AS120" s="10"/>
+      <c r="AS120" s="8"/>
     </row>
     <row r="121" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
@@ -9061,7 +9014,7 @@
       <c r="AR121" t="s">
         <v>416</v>
       </c>
-      <c r="AS121" s="10"/>
+      <c r="AS121" s="8"/>
     </row>
     <row r="122" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
@@ -9097,7 +9050,7 @@
       <c r="AR122" t="s">
         <v>417</v>
       </c>
-      <c r="AS122" s="10"/>
+      <c r="AS122" s="8"/>
     </row>
     <row r="123" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
@@ -9133,7 +9086,7 @@
       <c r="AR123" t="s">
         <v>418</v>
       </c>
-      <c r="AS123" s="10"/>
+      <c r="AS123" s="8"/>
     </row>
     <row r="124" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
@@ -9169,7 +9122,7 @@
       <c r="AR124" t="s">
         <v>419</v>
       </c>
-      <c r="AS124" s="10"/>
+      <c r="AS124" s="8"/>
     </row>
     <row r="125" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
@@ -9205,7 +9158,7 @@
       <c r="AR125" t="s">
         <v>420</v>
       </c>
-      <c r="AS125" s="10"/>
+      <c r="AS125" s="8"/>
     </row>
     <row r="126" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
@@ -9241,7 +9194,7 @@
       <c r="AR126" t="s">
         <v>421</v>
       </c>
-      <c r="AS126" s="10"/>
+      <c r="AS126" s="8"/>
     </row>
     <row r="127" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
@@ -9277,7 +9230,7 @@
       <c r="AR127" t="s">
         <v>422</v>
       </c>
-      <c r="AS127" s="10"/>
+      <c r="AS127" s="8"/>
     </row>
     <row r="128" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
@@ -9313,7 +9266,7 @@
       <c r="AR128" t="s">
         <v>423</v>
       </c>
-      <c r="AS128" s="10"/>
+      <c r="AS128" s="8"/>
     </row>
     <row r="129" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
@@ -9349,7 +9302,7 @@
       <c r="AR129" t="s">
         <v>424</v>
       </c>
-      <c r="AS129" s="10"/>
+      <c r="AS129" s="8"/>
     </row>
     <row r="130" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
@@ -9385,7 +9338,7 @@
       <c r="AR130" t="s">
         <v>425</v>
       </c>
-      <c r="AS130" s="10"/>
+      <c r="AS130" s="8"/>
     </row>
     <row r="131" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
@@ -9421,7 +9374,7 @@
       <c r="AR131" t="s">
         <v>426</v>
       </c>
-      <c r="AS131" s="10"/>
+      <c r="AS131" s="8"/>
     </row>
     <row r="132" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
@@ -9457,7 +9410,7 @@
       <c r="AR132" t="s">
         <v>427</v>
       </c>
-      <c r="AS132" s="10"/>
+      <c r="AS132" s="8"/>
     </row>
     <row r="133" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
@@ -9493,7 +9446,7 @@
       <c r="AR133" t="s">
         <v>428</v>
       </c>
-      <c r="AS133" s="10"/>
+      <c r="AS133" s="8"/>
     </row>
     <row r="134" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
@@ -9529,7 +9482,7 @@
       <c r="AR134" t="s">
         <v>429</v>
       </c>
-      <c r="AS134" s="10"/>
+      <c r="AS134" s="8"/>
     </row>
     <row r="135" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
@@ -9565,7 +9518,7 @@
       <c r="AR135" t="s">
         <v>430</v>
       </c>
-      <c r="AS135" s="10"/>
+      <c r="AS135" s="8"/>
     </row>
     <row r="136" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
@@ -9601,7 +9554,7 @@
       <c r="AR136" t="s">
         <v>431</v>
       </c>
-      <c r="AS136" s="10"/>
+      <c r="AS136" s="8"/>
     </row>
     <row r="137" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
@@ -9637,7 +9590,7 @@
       <c r="AR137" t="s">
         <v>432</v>
       </c>
-      <c r="AS137" s="10"/>
+      <c r="AS137" s="8"/>
     </row>
     <row r="138" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
@@ -9673,7 +9626,7 @@
       <c r="AR138" t="s">
         <v>433</v>
       </c>
-      <c r="AS138" s="10"/>
+      <c r="AS138" s="8"/>
     </row>
     <row r="139" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
@@ -9709,7 +9662,7 @@
       <c r="AR139" t="s">
         <v>434</v>
       </c>
-      <c r="AS139" s="10"/>
+      <c r="AS139" s="8"/>
     </row>
     <row r="140" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
@@ -9745,7 +9698,7 @@
       <c r="AR140" t="s">
         <v>435</v>
       </c>
-      <c r="AS140" s="10"/>
+      <c r="AS140" s="8"/>
     </row>
     <row r="141" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
@@ -9781,7 +9734,7 @@
       <c r="AR141" t="s">
         <v>436</v>
       </c>
-      <c r="AS141" s="10"/>
+      <c r="AS141" s="8"/>
     </row>
     <row r="142" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
@@ -9817,7 +9770,7 @@
       <c r="AR142" t="s">
         <v>437</v>
       </c>
-      <c r="AS142" s="10"/>
+      <c r="AS142" s="8"/>
     </row>
     <row r="143" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
@@ -9853,7 +9806,7 @@
       <c r="AR143" t="s">
         <v>438</v>
       </c>
-      <c r="AS143" s="10"/>
+      <c r="AS143" s="8"/>
     </row>
     <row r="144" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
@@ -9889,7 +9842,7 @@
       <c r="AR144" t="s">
         <v>439</v>
       </c>
-      <c r="AS144" s="10"/>
+      <c r="AS144" s="8"/>
     </row>
     <row r="145" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
@@ -9925,7 +9878,7 @@
       <c r="AR145" t="s">
         <v>440</v>
       </c>
-      <c r="AS145" s="10"/>
+      <c r="AS145" s="8"/>
     </row>
     <row r="146" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
@@ -9961,7 +9914,7 @@
       <c r="AR146" t="s">
         <v>441</v>
       </c>
-      <c r="AS146" s="10"/>
+      <c r="AS146" s="8"/>
     </row>
     <row r="147" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
@@ -9997,7 +9950,7 @@
       <c r="AR147" t="s">
         <v>442</v>
       </c>
-      <c r="AS147" s="10"/>
+      <c r="AS147" s="8"/>
     </row>
     <row r="148" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
@@ -10033,7 +9986,7 @@
       <c r="AR148" t="s">
         <v>443</v>
       </c>
-      <c r="AS148" s="10"/>
+      <c r="AS148" s="8"/>
     </row>
     <row r="149" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
@@ -10069,7 +10022,7 @@
       <c r="AR149" t="s">
         <v>444</v>
       </c>
-      <c r="AS149" s="10"/>
+      <c r="AS149" s="8"/>
     </row>
     <row r="150" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
@@ -10105,7 +10058,7 @@
       <c r="AR150" t="s">
         <v>445</v>
       </c>
-      <c r="AS150" s="10"/>
+      <c r="AS150" s="8"/>
     </row>
     <row r="151" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
@@ -10141,7 +10094,7 @@
       <c r="AR151" t="s">
         <v>446</v>
       </c>
-      <c r="AS151" s="10"/>
+      <c r="AS151" s="8"/>
     </row>
     <row r="152" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
@@ -10177,7 +10130,7 @@
       <c r="AR152" t="s">
         <v>447</v>
       </c>
-      <c r="AS152" s="10"/>
+      <c r="AS152" s="8"/>
     </row>
     <row r="153" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
@@ -10213,7 +10166,7 @@
       <c r="AR153" t="s">
         <v>448</v>
       </c>
-      <c r="AS153" s="10"/>
+      <c r="AS153" s="8"/>
     </row>
     <row r="154" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
@@ -10249,7 +10202,7 @@
       <c r="AR154" t="s">
         <v>449</v>
       </c>
-      <c r="AS154" s="10"/>
+      <c r="AS154" s="8"/>
     </row>
     <row r="155" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
@@ -10285,7 +10238,7 @@
       <c r="AR155" t="s">
         <v>450</v>
       </c>
-      <c r="AS155" s="10"/>
+      <c r="AS155" s="8"/>
     </row>
     <row r="156" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
@@ -10321,7 +10274,7 @@
       <c r="AR156" t="s">
         <v>451</v>
       </c>
-      <c r="AS156" s="10"/>
+      <c r="AS156" s="8"/>
     </row>
     <row r="157" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
@@ -10357,7 +10310,7 @@
       <c r="AR157" t="s">
         <v>452</v>
       </c>
-      <c r="AS157" s="10"/>
+      <c r="AS157" s="8"/>
     </row>
     <row r="158" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
@@ -10393,7 +10346,7 @@
       <c r="AR158" t="s">
         <v>453</v>
       </c>
-      <c r="AS158" s="10"/>
+      <c r="AS158" s="8"/>
     </row>
     <row r="159" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
@@ -10429,7 +10382,7 @@
       <c r="AR159" t="s">
         <v>454</v>
       </c>
-      <c r="AS159" s="10"/>
+      <c r="AS159" s="8"/>
     </row>
     <row r="160" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
@@ -10465,7 +10418,7 @@
       <c r="AR160" t="s">
         <v>455</v>
       </c>
-      <c r="AS160" s="10"/>
+      <c r="AS160" s="8"/>
     </row>
     <row r="161" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
@@ -10501,7 +10454,7 @@
       <c r="AR161" t="s">
         <v>456</v>
       </c>
-      <c r="AS161" s="10"/>
+      <c r="AS161" s="8"/>
     </row>
     <row r="162" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
@@ -10537,7 +10490,7 @@
       <c r="AR162" t="s">
         <v>457</v>
       </c>
-      <c r="AS162" s="10"/>
+      <c r="AS162" s="8"/>
     </row>
     <row r="163" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
@@ -10573,7 +10526,7 @@
       <c r="AR163" t="s">
         <v>458</v>
       </c>
-      <c r="AS163" s="10"/>
+      <c r="AS163" s="8"/>
     </row>
     <row r="164" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
@@ -10609,7 +10562,7 @@
       <c r="AR164" t="s">
         <v>459</v>
       </c>
-      <c r="AS164" s="10"/>
+      <c r="AS164" s="8"/>
     </row>
     <row r="165" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
@@ -10645,7 +10598,7 @@
       <c r="AR165" t="s">
         <v>460</v>
       </c>
-      <c r="AS165" s="10"/>
+      <c r="AS165" s="8"/>
     </row>
     <row r="166" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
@@ -10681,7 +10634,7 @@
       <c r="AR166" t="s">
         <v>461</v>
       </c>
-      <c r="AS166" s="10"/>
+      <c r="AS166" s="8"/>
     </row>
     <row r="167" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
@@ -10717,7 +10670,7 @@
       <c r="AR167" t="s">
         <v>462</v>
       </c>
-      <c r="AS167" s="10"/>
+      <c r="AS167" s="8"/>
     </row>
     <row r="168" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
@@ -10753,7 +10706,7 @@
       <c r="AR168" t="s">
         <v>463</v>
       </c>
-      <c r="AS168" s="10"/>
+      <c r="AS168" s="8"/>
     </row>
     <row r="169" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
@@ -10789,7 +10742,7 @@
       <c r="AR169" t="s">
         <v>464</v>
       </c>
-      <c r="AS169" s="10"/>
+      <c r="AS169" s="8"/>
     </row>
     <row r="170" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
@@ -10825,7 +10778,7 @@
       <c r="AR170" t="s">
         <v>465</v>
       </c>
-      <c r="AS170" s="10"/>
+      <c r="AS170" s="8"/>
     </row>
     <row r="171" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
@@ -10861,7 +10814,7 @@
       <c r="AR171" t="s">
         <v>466</v>
       </c>
-      <c r="AS171" s="10"/>
+      <c r="AS171" s="8"/>
     </row>
     <row r="172" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
@@ -10897,7 +10850,7 @@
       <c r="AR172" t="s">
         <v>467</v>
       </c>
-      <c r="AS172" s="10"/>
+      <c r="AS172" s="8"/>
     </row>
     <row r="173" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
@@ -10933,7 +10886,7 @@
       <c r="AR173" t="s">
         <v>468</v>
       </c>
-      <c r="AS173" s="10"/>
+      <c r="AS173" s="8"/>
     </row>
     <row r="174" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
@@ -10969,7 +10922,7 @@
       <c r="AR174" t="s">
         <v>469</v>
       </c>
-      <c r="AS174" s="10"/>
+      <c r="AS174" s="8"/>
     </row>
     <row r="175" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
@@ -11005,13 +10958,13 @@
       <c r="AR175" t="s">
         <v>470</v>
       </c>
-      <c r="AS175" s="10"/>
+      <c r="AS175" s="8"/>
     </row>
     <row r="176" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>167</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B176" s="3" t="s">
         <v>185</v>
       </c>
       <c r="C176" t="b">
@@ -11041,13 +10994,13 @@
       <c r="AR176" t="s">
         <v>471</v>
       </c>
-      <c r="AS176" s="10"/>
+      <c r="AS176" s="8"/>
     </row>
     <row r="177" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>168</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="3" t="s">
         <v>189</v>
       </c>
       <c r="C177" t="b">
@@ -11077,13 +11030,13 @@
       <c r="AR177" t="s">
         <v>472</v>
       </c>
-      <c r="AS177" s="10"/>
+      <c r="AS177" s="8"/>
     </row>
     <row r="178" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>169</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B178" s="3" t="s">
         <v>186</v>
       </c>
       <c r="C178" t="b">
@@ -11113,13 +11066,13 @@
       <c r="AR178" t="s">
         <v>473</v>
       </c>
-      <c r="AS178" s="10"/>
+      <c r="AS178" s="8"/>
     </row>
     <row r="179" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>170</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B179" s="3" t="s">
         <v>187</v>
       </c>
       <c r="C179" t="b">
@@ -11149,13 +11102,13 @@
       <c r="AR179" t="s">
         <v>474</v>
       </c>
-      <c r="AS179" s="10"/>
+      <c r="AS179" s="8"/>
     </row>
     <row r="180" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>171</v>
       </c>
-      <c r="B180" s="4" t="s">
+      <c r="B180" s="3" t="s">
         <v>191</v>
       </c>
       <c r="C180" t="b">
@@ -11184,7 +11137,7 @@
       <c r="A181" s="1">
         <v>172</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B181" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C181" t="b">
@@ -11213,7 +11166,7 @@
       <c r="A182" s="1">
         <v>173</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B182" s="3" t="s">
         <v>188</v>
       </c>
       <c r="C182" t="b">
@@ -11242,7 +11195,7 @@
       <c r="A183" s="1">
         <v>174</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B183" s="3" t="s">
         <v>192</v>
       </c>
       <c r="C183" t="b">
@@ -11268,16 +11221,17 @@
       </c>
     </row>
     <row r="184" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="E184" s="4"/>
-      <c r="F184" s="4"/>
-      <c r="G184" s="4"/>
-      <c r="H184" s="4"/>
-      <c r="I184" s="4"/>
-      <c r="J184" s="4"/>
-      <c r="K184" s="4"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
+      <c r="H184" s="3"/>
+      <c r="I184" s="3"/>
+      <c r="J184" s="3"/>
+      <c r="K184" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AK8:AL8"/>
     <mergeCell ref="CJ8:CX8"/>
     <mergeCell ref="CG8:CH8"/>
     <mergeCell ref="CZ8:DJ8"/>
@@ -11294,10 +11248,49 @@
     <mergeCell ref="AQ8:AS8"/>
     <mergeCell ref="AD8:AE8"/>
     <mergeCell ref="AG8:AI8"/>
-    <mergeCell ref="AK8:AL8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA64165-0436-FF42-8A3B-26565227B56E}">
+  <dimension ref="A5:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>597</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>